<commit_message>
Spotipy to compute most common genres
</commit_message>
<xml_diff>
--- a/bands.xlsx
+++ b/bands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="536">
   <si>
     <t>7 Notas 7 Colores</t>
   </si>
@@ -857,6 +857,777 @@
   </si>
   <si>
     <t>","headLevel":"</t>
+  </si>
+  <si>
+    <t>alternative dance</t>
+  </si>
+  <si>
+    <t>dance-punk</t>
+  </si>
+  <si>
+    <t>electroclash</t>
+  </si>
+  <si>
+    <t>electronic</t>
+  </si>
+  <si>
+    <t>indie pop</t>
+  </si>
+  <si>
+    <t>indie rock</t>
+  </si>
+  <si>
+    <t>indietronica</t>
+  </si>
+  <si>
+    <t>new rave</t>
+  </si>
+  <si>
+    <t>synthpop</t>
+  </si>
+  <si>
+    <t>spanish hip hop</t>
+  </si>
+  <si>
+    <t>trap latino</t>
+  </si>
+  <si>
+    <t>dub techno</t>
+  </si>
+  <si>
+    <t>float house</t>
+  </si>
+  <si>
+    <t>mandible</t>
+  </si>
+  <si>
+    <t>minimal dub</t>
+  </si>
+  <si>
+    <t>outsider house</t>
+  </si>
+  <si>
+    <t>alternative pop</t>
+  </si>
+  <si>
+    <t>alternative rock</t>
+  </si>
+  <si>
+    <t>dream pop</t>
+  </si>
+  <si>
+    <t>grunge</t>
+  </si>
+  <si>
+    <t>lo-fi</t>
+  </si>
+  <si>
+    <t>permanent wave</t>
+  </si>
+  <si>
+    <t>post-hardcore</t>
+  </si>
+  <si>
+    <t>power pop</t>
+  </si>
+  <si>
+    <t>slow core</t>
+  </si>
+  <si>
+    <t>space rock</t>
+  </si>
+  <si>
+    <t>anti-folk</t>
+  </si>
+  <si>
+    <t>emo</t>
+  </si>
+  <si>
+    <t>folk punk</t>
+  </si>
+  <si>
+    <t>melodic hardcore</t>
+  </si>
+  <si>
+    <t>orgcore</t>
+  </si>
+  <si>
+    <t>pop punk</t>
+  </si>
+  <si>
+    <t>punk</t>
+  </si>
+  <si>
+    <t>skate punk</t>
+  </si>
+  <si>
+    <t>deep latin hip hop</t>
+  </si>
+  <si>
+    <t>australian alternative rock</t>
+  </si>
+  <si>
+    <t>alt-indie rock</t>
+  </si>
+  <si>
+    <t>chamber psych</t>
+  </si>
+  <si>
+    <t>spanish noise pop</t>
+  </si>
+  <si>
+    <t>chamber pop</t>
+  </si>
+  <si>
+    <t>escape room</t>
+  </si>
+  <si>
+    <t>folk-pop</t>
+  </si>
+  <si>
+    <t>freak folk</t>
+  </si>
+  <si>
+    <t>garage psych</t>
+  </si>
+  <si>
+    <t>indie folk</t>
+  </si>
+  <si>
+    <t>indie r&amp;b</t>
+  </si>
+  <si>
+    <t>neo-psychedelic</t>
+  </si>
+  <si>
+    <t>noise pop</t>
+  </si>
+  <si>
+    <t>preverb</t>
+  </si>
+  <si>
+    <t>singer-songwriter</t>
+  </si>
+  <si>
+    <t>stomp and holler</t>
+  </si>
+  <si>
+    <t>anime</t>
+  </si>
+  <si>
+    <t>free improvisation</t>
+  </si>
+  <si>
+    <t>free jazz</t>
+  </si>
+  <si>
+    <t>acid techno</t>
+  </si>
+  <si>
+    <t>ambient</t>
+  </si>
+  <si>
+    <t>drill and bass</t>
+  </si>
+  <si>
+    <t>fourth world</t>
+  </si>
+  <si>
+    <t>intelligent dance music</t>
+  </si>
+  <si>
+    <t>microhouse</t>
+  </si>
+  <si>
+    <t>trip hop</t>
+  </si>
+  <si>
+    <t>canadian indie</t>
+  </si>
+  <si>
+    <t>canadian pop</t>
+  </si>
+  <si>
+    <t>garage rock</t>
+  </si>
+  <si>
+    <t>jungle</t>
+  </si>
+  <si>
+    <t>detroit techno</t>
+  </si>
+  <si>
+    <t>fluxwork</t>
+  </si>
+  <si>
+    <t>alternative hip hop</t>
+  </si>
+  <si>
+    <t>dark jazz</t>
+  </si>
+  <si>
+    <t>hip hop</t>
+  </si>
+  <si>
+    <t>soul</t>
+  </si>
+  <si>
+    <t>spanish indie pop</t>
+  </si>
+  <si>
+    <t>bubble trance</t>
+  </si>
+  <si>
+    <t>basque rock</t>
+  </si>
+  <si>
+    <t>spanish punk</t>
+  </si>
+  <si>
+    <t>deep disco house</t>
+  </si>
+  <si>
+    <t>deep groove house</t>
+  </si>
+  <si>
+    <t>deep house</t>
+  </si>
+  <si>
+    <t>disco house</t>
+  </si>
+  <si>
+    <t>future garage</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>minimal tech house</t>
+  </si>
+  <si>
+    <t>tech house</t>
+  </si>
+  <si>
+    <t>uk garage</t>
+  </si>
+  <si>
+    <t>blues-rock</t>
+  </si>
+  <si>
+    <t>modern blues</t>
+  </si>
+  <si>
+    <t>nu gaze</t>
+  </si>
+  <si>
+    <t>psychedelic rock</t>
+  </si>
+  <si>
+    <t>punk blues</t>
+  </si>
+  <si>
+    <t>melancholia</t>
+  </si>
+  <si>
+    <t>neo mellow</t>
+  </si>
+  <si>
+    <t>chillwave</t>
+  </si>
+  <si>
+    <t>experimental rock</t>
+  </si>
+  <si>
+    <t>noise rock</t>
+  </si>
+  <si>
+    <t>post rock</t>
+  </si>
+  <si>
+    <t>shimmer pop</t>
+  </si>
+  <si>
+    <t>mexican indie</t>
+  </si>
+  <si>
+    <t>chaotic hardcore</t>
+  </si>
+  <si>
+    <t>grindcore</t>
+  </si>
+  <si>
+    <t>jazz metal</t>
+  </si>
+  <si>
+    <t>math rock</t>
+  </si>
+  <si>
+    <t>mathcore</t>
+  </si>
+  <si>
+    <t>metalcore</t>
+  </si>
+  <si>
+    <t>post-doom metal</t>
+  </si>
+  <si>
+    <t>post-metal</t>
+  </si>
+  <si>
+    <t>screamo</t>
+  </si>
+  <si>
+    <t>sludge metal</t>
+  </si>
+  <si>
+    <t>straight edge</t>
+  </si>
+  <si>
+    <t>brooklyn indie</t>
+  </si>
+  <si>
+    <t>indie punk</t>
+  </si>
+  <si>
+    <t>dance rock</t>
+  </si>
+  <si>
+    <t>gothic rock</t>
+  </si>
+  <si>
+    <t>hardcore punk</t>
+  </si>
+  <si>
+    <t>industrial rock</t>
+  </si>
+  <si>
+    <t>new wave</t>
+  </si>
+  <si>
+    <t>no wave</t>
+  </si>
+  <si>
+    <t>post-punk</t>
+  </si>
+  <si>
+    <t>pub rock</t>
+  </si>
+  <si>
+    <t>uk post-punk</t>
+  </si>
+  <si>
+    <t>underground hip hop</t>
+  </si>
+  <si>
+    <t>vaporwave</t>
+  </si>
+  <si>
+    <t>ska</t>
+  </si>
+  <si>
+    <t>ska punk</t>
+  </si>
+  <si>
+    <t>cantautor</t>
+  </si>
+  <si>
+    <t>rock catala</t>
+  </si>
+  <si>
+    <t>bossa nova</t>
+  </si>
+  <si>
+    <t>brazilian indie</t>
+  </si>
+  <si>
+    <t>forro</t>
+  </si>
+  <si>
+    <t>mpb</t>
+  </si>
+  <si>
+    <t>pagode</t>
+  </si>
+  <si>
+    <t>samba</t>
+  </si>
+  <si>
+    <t>velha guarda</t>
+  </si>
+  <si>
+    <t>deep indie rock</t>
+  </si>
+  <si>
+    <t>glitch</t>
+  </si>
+  <si>
+    <t>glitch hop</t>
+  </si>
+  <si>
+    <t>wonky</t>
+  </si>
+  <si>
+    <t>dance pop</t>
+  </si>
+  <si>
+    <t>neo soul</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>pop rap</t>
+  </si>
+  <si>
+    <t>rap</t>
+  </si>
+  <si>
+    <t>dark wave</t>
+  </si>
+  <si>
+    <t>ebm</t>
+  </si>
+  <si>
+    <t>electro-industrial</t>
+  </si>
+  <si>
+    <t>experimental</t>
+  </si>
+  <si>
+    <t>futurepop</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>industrial metal</t>
+  </si>
+  <si>
+    <t>new beat</t>
+  </si>
+  <si>
+    <t>new romantic</t>
+  </si>
+  <si>
+    <t>drone</t>
+  </si>
+  <si>
+    <t>minimal</t>
+  </si>
+  <si>
+    <t>gauze pop</t>
+  </si>
+  <si>
+    <t>shiver pop</t>
+  </si>
+  <si>
+    <t>alternative metal</t>
+  </si>
+  <si>
+    <t>death metal</t>
+  </si>
+  <si>
+    <t>groove metal</t>
+  </si>
+  <si>
+    <t>melodic metalcore</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>nu metal</t>
+  </si>
+  <si>
+    <t>progressive metal</t>
+  </si>
+  <si>
+    <t>nu disco</t>
+  </si>
+  <si>
+    <t>deep australian indie</t>
+  </si>
+  <si>
+    <t>art rock</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>new wave pop</t>
+  </si>
+  <si>
+    <t>britpop</t>
+  </si>
+  <si>
+    <t>e6fi</t>
+  </si>
+  <si>
+    <t>indie garage rock</t>
+  </si>
+  <si>
+    <t>minimal techno</t>
+  </si>
+  <si>
+    <t>bass music</t>
+  </si>
+  <si>
+    <t>deep euro house</t>
+  </si>
+  <si>
+    <t>deep melodic euro house</t>
+  </si>
+  <si>
+    <t>tropical house</t>
+  </si>
+  <si>
+    <t>italian indie pop</t>
+  </si>
+  <si>
+    <t>spanish indie rock</t>
+  </si>
+  <si>
+    <t>vancouver indie</t>
+  </si>
+  <si>
+    <t>balearic</t>
+  </si>
+  <si>
+    <t>new weird america</t>
+  </si>
+  <si>
+    <t>spanish folk</t>
+  </si>
+  <si>
+    <t>new americana</t>
+  </si>
+  <si>
+    <t>roots rock</t>
+  </si>
+  <si>
+    <t>compositional ambient</t>
+  </si>
+  <si>
+    <t>icelandic pop</t>
+  </si>
+  <si>
+    <t>techno</t>
+  </si>
+  <si>
+    <t>funk</t>
+  </si>
+  <si>
+    <t>deep soul house</t>
+  </si>
+  <si>
+    <t>indie poptimism</t>
+  </si>
+  <si>
+    <t>indie psych-rock</t>
+  </si>
+  <si>
+    <t>la indie</t>
+  </si>
+  <si>
+    <t>alternative emo</t>
+  </si>
+  <si>
+    <t>metropopolis</t>
+  </si>
+  <si>
+    <t>twee pop</t>
+  </si>
+  <si>
+    <t>grave wave</t>
+  </si>
+  <si>
+    <t>french indietronica</t>
+  </si>
+  <si>
+    <t>hip pop</t>
+  </si>
+  <si>
+    <t>r&amp;b</t>
+  </si>
+  <si>
+    <t>trap music</t>
+  </si>
+  <si>
+    <t>urban contemporary</t>
+  </si>
+  <si>
+    <t>alternative country</t>
+  </si>
+  <si>
+    <t>country rock</t>
+  </si>
+  <si>
+    <t>deep new americana</t>
+  </si>
+  <si>
+    <t>aussietronica</t>
+  </si>
+  <si>
+    <t>garage pop</t>
+  </si>
+  <si>
+    <t>dubstep</t>
+  </si>
+  <si>
+    <t>afrobeat</t>
+  </si>
+  <si>
+    <t>indie jazz</t>
+  </si>
+  <si>
+    <t>ninja</t>
+  </si>
+  <si>
+    <t>retro electro</t>
+  </si>
+  <si>
+    <t>big beat</t>
+  </si>
+  <si>
+    <t>indie christmas</t>
+  </si>
+  <si>
+    <t>madchester</t>
+  </si>
+  <si>
+    <t>deep indie r&amp;b</t>
+  </si>
+  <si>
+    <t>chicago indie</t>
+  </si>
+  <si>
+    <t>gbvfi</t>
+  </si>
+  <si>
+    <t>grime</t>
+  </si>
+  <si>
+    <t>digital hardcore</t>
+  </si>
+  <si>
+    <t>album rock</t>
+  </si>
+  <si>
+    <t>hard rock</t>
+  </si>
+  <si>
+    <t>rap metal</t>
+  </si>
+  <si>
+    <t>rap rock</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>speed metal</t>
+  </si>
+  <si>
+    <t>thrash metal</t>
+  </si>
+  <si>
+    <t>doom metal</t>
+  </si>
+  <si>
+    <t>drone metal</t>
+  </si>
+  <si>
+    <t>psychedelic doom</t>
+  </si>
+  <si>
+    <t>stoner metal</t>
+  </si>
+  <si>
+    <t>stoner rock</t>
+  </si>
+  <si>
+    <t>gothic americana</t>
+  </si>
+  <si>
+    <t>pop christmas</t>
+  </si>
+  <si>
+    <t>shoegaze</t>
+  </si>
+  <si>
+    <t>jangle pop</t>
+  </si>
+  <si>
+    <t>pop rock</t>
+  </si>
+  <si>
+    <t>scottish rock</t>
+  </si>
+  <si>
+    <t>spanish new wave</t>
+  </si>
+  <si>
+    <t>downtempo</t>
+  </si>
+  <si>
+    <t>classic rock</t>
+  </si>
+  <si>
+    <t>folk</t>
+  </si>
+  <si>
+    <t>folk rock</t>
+  </si>
+  <si>
+    <t>mellow gold</t>
+  </si>
+  <si>
+    <t>soft rock</t>
+  </si>
+  <si>
+    <t>folk christmas</t>
+  </si>
+  <si>
+    <t>c86</t>
+  </si>
+  <si>
+    <t>leeds indie</t>
+  </si>
+  <si>
+    <t>drone folk</t>
+  </si>
+  <si>
+    <t>brill building pop</t>
+  </si>
+  <si>
+    <t>british blues</t>
+  </si>
+  <si>
+    <t>british invasion</t>
+  </si>
+  <si>
+    <t>bubblegum pop</t>
+  </si>
+  <si>
+    <t>classic funk rock</t>
+  </si>
+  <si>
+    <t>kiwi rock</t>
+  </si>
+  <si>
+    <t>nz indie</t>
+  </si>
+  <si>
+    <t>chilean rock</t>
+  </si>
+  <si>
+    <t>rock gaucho</t>
+  </si>
+  <si>
+    <t>peruvian rock</t>
+  </si>
+  <si>
+    <t>indie</t>
   </si>
 </sst>
 </file>
@@ -923,8 +1694,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1024,7 +1797,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1068,6 +1841,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1111,6 +1885,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1442,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A259" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -10953,7 +11728,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10964,13 +11738,1324 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C256"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>535</v>
+      </c>
+      <c r="C7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>534</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>